<commit_message>
Added usd rate column
</commit_message>
<xml_diff>
--- a/sheets/example.xlsx
+++ b/sheets/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="555" windowWidth="24615" windowHeight="8895"/>
+    <workbookView xWindow="360" yWindow="585" windowWidth="21735" windowHeight="9405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prices" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Дата/Продукт</t>
   </si>
@@ -32,10 +32,28 @@
     <t>LG F-80C3LD</t>
   </si>
   <si>
+    <t>Сумма</t>
+  </si>
+  <si>
+    <t>Курс $</t>
+  </si>
+  <si>
     <t>Наименование</t>
   </si>
   <si>
     <t>Код</t>
+  </si>
+  <si>
+    <t>холодильник</t>
+  </si>
+  <si>
+    <t>варочная поверхность</t>
+  </si>
+  <si>
+    <t>дух. Шкаф</t>
+  </si>
+  <si>
+    <t>стиралка</t>
   </si>
 </sst>
 </file>
@@ -96,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -106,6 +124,15 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -402,11 +429,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L870"/>
+  <dimension ref="A1:M870"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -416,9 +443,11 @@
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29.25" customHeight="1">
+    <row r="1" spans="1:13" ht="29.25" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -440,9 +469,14 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="L1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="5">
         <v>42094.462766204</v>
       </c>
@@ -464,9 +498,12 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="L2" s="2">
+        <f t="shared" ref="L2:L65" si="0">IF(SUM(B2:K2)=0,"",SUM(B2:K2))</f>
+        <v>69314.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="5">
         <v>42102.378750000003</v>
       </c>
@@ -488,9 +525,12 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="L3" s="2">
+        <f t="shared" si="0"/>
+        <v>69690</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="5">
         <v>42103.306030093001</v>
       </c>
@@ -512,9 +552,12 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="L4" s="2">
+        <f t="shared" si="0"/>
+        <v>69683</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="5">
         <v>42104.570868055998</v>
       </c>
@@ -536,9 +579,12 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="L5" s="2">
+        <f t="shared" si="0"/>
+        <v>72542.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="5">
         <v>42106.281666666997</v>
       </c>
@@ -560,9 +606,12 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="2">
+        <f t="shared" si="0"/>
+        <v>73965</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="5">
         <v>42107.512129629999</v>
       </c>
@@ -584,289 +633,555 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="L7" s="2">
+        <f t="shared" si="0"/>
+        <v>64973</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="5">
+        <v>42108.306006944003</v>
+      </c>
+      <c r="B8" s="2">
+        <v>17940</v>
+      </c>
+      <c r="C8" s="2">
+        <v>14460</v>
+      </c>
+      <c r="D8" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E8" s="2">
+        <v>17600</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="L8" s="2">
+        <f t="shared" si="0"/>
+        <v>64880</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="5">
+        <v>42109.276840277998</v>
+      </c>
+      <c r="B9" s="2">
+        <v>18010</v>
+      </c>
+      <c r="C9" s="2">
+        <v>14439</v>
+      </c>
+      <c r="D9" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E9" s="2">
+        <v>17542</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="L9" s="2">
+        <f t="shared" si="0"/>
+        <v>64871</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="5">
+        <v>42110.285833333</v>
+      </c>
+      <c r="B10" s="2">
+        <v>18189</v>
+      </c>
+      <c r="C10" s="2">
+        <v>14439</v>
+      </c>
+      <c r="D10" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E10" s="2">
+        <v>17268</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="3"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="L10" s="2">
+        <f t="shared" si="0"/>
+        <v>64776</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="5">
+        <v>42111.306041666998</v>
+      </c>
+      <c r="B11" s="2">
+        <v>18010</v>
+      </c>
+      <c r="C11" s="2">
+        <v>14439</v>
+      </c>
+      <c r="D11" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E11" s="2">
+        <v>17227</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="L11" s="2">
+        <f t="shared" si="0"/>
+        <v>64556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="5">
+        <v>42114.307013889003</v>
+      </c>
+      <c r="B12" s="2">
+        <v>18200</v>
+      </c>
+      <c r="C12" s="2">
+        <v>14441</v>
+      </c>
+      <c r="D12" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E12" s="2">
+        <v>17227</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="L12" s="2">
+        <f t="shared" si="0"/>
+        <v>64748</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="5">
+        <v>42115.306041666998</v>
+      </c>
+      <c r="B13" s="2">
+        <v>18547</v>
+      </c>
+      <c r="C13" s="2">
+        <v>14441</v>
+      </c>
+      <c r="D13" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E13" s="2">
+        <v>17350</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="L13" s="2">
+        <f t="shared" si="0"/>
+        <v>65218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="5">
+        <v>42116.305960648002</v>
+      </c>
+      <c r="B14" s="2">
+        <v>18410</v>
+      </c>
+      <c r="C14" s="2">
+        <v>14439</v>
+      </c>
+      <c r="D14" s="2">
+        <v>15605</v>
+      </c>
+      <c r="E14" s="2">
+        <v>17390</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="L14" s="2">
+        <f t="shared" si="0"/>
+        <v>65844</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="5">
+        <v>42117.305995369999</v>
+      </c>
+      <c r="B15" s="2">
+        <v>18451</v>
+      </c>
+      <c r="C15" s="2">
+        <v>14253</v>
+      </c>
+      <c r="D15" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E15" s="2">
+        <v>17330</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="3"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="L15" s="2">
+        <f t="shared" si="0"/>
+        <v>64914</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="5">
+        <v>42118.306030093001</v>
+      </c>
+      <c r="B16" s="2">
+        <v>18365</v>
+      </c>
+      <c r="C16" s="2">
+        <v>13985</v>
+      </c>
+      <c r="D16" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E16" s="2">
+        <v>17350</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="3"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="L16" s="2">
+        <f t="shared" si="0"/>
+        <v>64580</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="5">
+        <v>42120.814050925997</v>
+      </c>
+      <c r="B17" s="2">
+        <v>18499</v>
+      </c>
+      <c r="C17" s="2">
+        <v>13890</v>
+      </c>
+      <c r="D17" s="2">
+        <v>14873</v>
+      </c>
+      <c r="E17" s="2">
+        <v>17548</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="3"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="L17" s="2">
+        <f t="shared" si="0"/>
+        <v>64810</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="5">
+        <v>42121.305995369999</v>
+      </c>
+      <c r="B18" s="2">
+        <v>18410</v>
+      </c>
+      <c r="C18" s="2">
+        <v>13810</v>
+      </c>
+      <c r="D18" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E18" s="2">
+        <v>17310</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="3"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="L18" s="2">
+        <f t="shared" si="0"/>
+        <v>64410</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="5">
+        <v>42122.306238425997</v>
+      </c>
+      <c r="B19" s="2">
+        <v>17994</v>
+      </c>
+      <c r="C19" s="2">
+        <v>13615</v>
+      </c>
+      <c r="D19" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E19" s="2">
+        <v>17310</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="3"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="L19" s="2">
+        <f t="shared" si="0"/>
+        <v>63799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="5">
+        <v>42123.306041666998</v>
+      </c>
+      <c r="B20" s="2">
+        <v>18365</v>
+      </c>
+      <c r="C20" s="2">
+        <v>13640</v>
+      </c>
+      <c r="D20" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E20" s="2">
+        <v>17310</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="3"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="L20" s="2">
+        <f t="shared" si="0"/>
+        <v>64195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="5">
+        <v>42124.306041666998</v>
+      </c>
+      <c r="B21" s="2">
+        <v>18055</v>
+      </c>
+      <c r="C21" s="2">
+        <v>13810</v>
+      </c>
+      <c r="D21" s="2">
+        <v>14880</v>
+      </c>
+      <c r="E21" s="2">
+        <v>17385</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="3"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="L21" s="2">
+        <f t="shared" si="0"/>
+        <v>64130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="5">
+        <v>42129.306030093001</v>
+      </c>
+      <c r="B22" s="2">
+        <v>18109</v>
+      </c>
+      <c r="C22" s="2">
+        <v>13561</v>
+      </c>
+      <c r="D22" s="2">
+        <v>14873</v>
+      </c>
+      <c r="E22" s="2">
+        <v>17225</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="3"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="L22" s="2">
+        <f t="shared" si="0"/>
+        <v>63768</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="5">
+        <v>42130.306030093001</v>
+      </c>
+      <c r="B23" s="2">
+        <v>18547</v>
+      </c>
+      <c r="C23" s="2">
+        <v>13610</v>
+      </c>
+      <c r="D23" s="2">
+        <v>14873</v>
+      </c>
+      <c r="E23" s="2">
+        <v>17310</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="3"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="L23" s="2">
+        <f t="shared" si="0"/>
+        <v>64340</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="5">
+        <v>42131.306030093001</v>
+      </c>
+      <c r="B24" s="2">
+        <v>17950</v>
+      </c>
+      <c r="C24" s="2">
+        <v>13170</v>
+      </c>
+      <c r="D24" s="2">
+        <v>14873</v>
+      </c>
+      <c r="E24" s="2">
+        <v>17197</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="3"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="L24" s="2">
+        <f t="shared" si="0"/>
+        <v>63190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="5">
+        <v>42132.306041666998</v>
+      </c>
+      <c r="B25" s="2">
+        <v>18055</v>
+      </c>
+      <c r="C25" s="2">
+        <v>13389</v>
+      </c>
+      <c r="D25" s="2">
+        <v>14873</v>
+      </c>
+      <c r="E25" s="2">
+        <v>17225</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="3"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="L25" s="2">
+        <f t="shared" si="0"/>
+        <v>63542</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="5">
+        <v>42135.306041666998</v>
+      </c>
+      <c r="B26" s="2">
+        <v>17900</v>
+      </c>
+      <c r="C26" s="2">
+        <v>13350</v>
+      </c>
+      <c r="D26" s="2">
+        <v>14873</v>
+      </c>
+      <c r="E26" s="2">
+        <v>17135</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="3"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="L26" s="2">
+        <f t="shared" si="0"/>
+        <v>63258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="5">
+        <v>42136.488344906997</v>
+      </c>
+      <c r="B27" s="2">
+        <v>17900</v>
+      </c>
+      <c r="C27" s="2">
+        <v>13350</v>
+      </c>
+      <c r="D27" s="2">
+        <v>14873</v>
+      </c>
+      <c r="E27" s="2">
+        <v>17197</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="L27" s="2">
+        <f t="shared" si="0"/>
+        <v>63320</v>
+      </c>
+      <c r="M27">
+        <v>50.914000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -878,9 +1193,12 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="L28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -892,9 +1210,12 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="L29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -906,9 +1227,12 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="L30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="3"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -920,9 +1244,12 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="L31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="3"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -934,7 +1261,10 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
+      <c r="L32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3"/>
@@ -948,7 +1278,10 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="L33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3"/>
@@ -962,7 +1295,10 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
+      <c r="L34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3"/>
@@ -976,7 +1312,10 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
+      <c r="L35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="3"/>
@@ -990,7 +1329,10 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
+      <c r="L36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="3"/>
@@ -1004,7 +1346,10 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
+      <c r="L37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="3"/>
@@ -1018,7 +1363,10 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
+      <c r="L38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="3"/>
@@ -1032,7 +1380,10 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
+      <c r="L39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="3"/>
@@ -1046,7 +1397,10 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
+      <c r="L40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="3"/>
@@ -1060,7 +1414,10 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
+      <c r="L41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3"/>
@@ -1074,7 +1431,10 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
+      <c r="L42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="3"/>
@@ -1088,7 +1448,10 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
+      <c r="L43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="3"/>
@@ -1102,7 +1465,10 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
+      <c r="L44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="3"/>
@@ -1116,7 +1482,10 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
+      <c r="L45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="3"/>
@@ -1130,7 +1499,10 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
+      <c r="L46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="3"/>
@@ -1144,7 +1516,10 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
+      <c r="L47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="3"/>
@@ -1158,7 +1533,10 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
+      <c r="L48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="3"/>
@@ -1172,7 +1550,10 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
+      <c r="L49" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3"/>
@@ -1186,7 +1567,10 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
+      <c r="L50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="3"/>
@@ -1200,7 +1584,10 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
+      <c r="L51" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="3"/>
@@ -1214,7 +1601,10 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
+      <c r="L52" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="3"/>
@@ -1228,7 +1618,10 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
+      <c r="L53" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="3"/>
@@ -1242,7 +1635,10 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
+      <c r="L54" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="3"/>
@@ -1256,7 +1652,10 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
+      <c r="L55" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="3"/>
@@ -1270,7 +1669,10 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
+      <c r="L56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="3"/>
@@ -1284,7 +1686,10 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
+      <c r="L57" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3"/>
@@ -1298,7 +1703,10 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
+      <c r="L58" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="3"/>
@@ -1312,7 +1720,10 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
+      <c r="L59" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="3"/>
@@ -1326,7 +1737,10 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
+      <c r="L60" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="3"/>
@@ -1340,7 +1754,10 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
+      <c r="L61" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="3"/>
@@ -1354,7 +1771,10 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
+      <c r="L62" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="3"/>
@@ -1368,7 +1788,10 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
+      <c r="L63" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="3"/>
@@ -1382,7 +1805,10 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
+      <c r="L64" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="3"/>
@@ -1396,7 +1822,10 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
+      <c r="L65" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3"/>
@@ -1410,7 +1839,10 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
+      <c r="L66" s="2" t="str">
+        <f t="shared" ref="L66:L67" si="1">IF(SUM(B66:K66)=0,"",SUM(B66:K66))</f>
+        <v/>
+      </c>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="3"/>
@@ -1424,7 +1856,10 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
+      <c r="L67" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="3"/>
@@ -8301,23 +8736,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="97.140625" customWidth="1"/>
+    <col min="4" max="4" width="60.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -8334,6 +8770,9 @@
         <f t="shared" ref="D2:D27" si="0">IF(ISBLANK(B2),"",HYPERLINK("http://market.yandex.ru/product/"&amp;B2&amp;"/"))</f>
         <v>http://market.yandex.ru/product/7747365/</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -8346,6 +8785,9 @@
         <f t="shared" si="0"/>
         <v>http://market.yandex.ru/product/8229520/</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -8358,6 +8800,9 @@
         <f t="shared" si="0"/>
         <v>http://market.yandex.ru/product/6290942/</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -8369,6 +8814,9 @@
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>http://market.yandex.ru/product/9275006/</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5">

</xml_diff>